<commit_message>
Deliverables Checklist update 20130628
</commit_message>
<xml_diff>
--- a/LEGO_Deliverables_Checklist.xlsx
+++ b/LEGO_Deliverables_Checklist.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="23206"/>
   <workbookPr hidePivotFieldList="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="28100" yWindow="-4180" windowWidth="25600" windowHeight="15480"/>
+    <workbookView xWindow="12880" yWindow="0" windowWidth="12720" windowHeight="15480"/>
   </bookViews>
   <sheets>
     <sheet name="FishTank Deliverables" sheetId="1" r:id="rId1"/>
@@ -82,7 +82,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1265" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1267" uniqueCount="342">
   <si>
     <t>TBD</t>
   </si>
@@ -2199,6 +2199,21 @@
     <xf numFmtId="0" fontId="19" fillId="9" borderId="5" xfId="224" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="35" fillId="10" borderId="1" xfId="224" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="10" borderId="1" xfId="224" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="35" fillId="10" borderId="1" xfId="224" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="35" fillId="10" borderId="1" xfId="224" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2216,21 +2231,6 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="10" borderId="1" xfId="224" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="10" borderId="1" xfId="224" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="35" fillId="10" borderId="1" xfId="224" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="10" borderId="1" xfId="224" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="297">
@@ -2532,303 +2532,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" customBuiltin="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="279">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749992370372631"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749992370372631"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
+  <dxfs count="181">
     <dxf>
       <fill>
         <patternFill>
@@ -3814,6 +3518,154 @@
     </dxf>
     <dxf>
       <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="-0.24994659260841701"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <color theme="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.39994506668294322"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor theme="4" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C6500"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFEB9C"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="3"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="3" tint="0.79998168889431442"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="2" tint="-0.749992370372631"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
         <color rgb="FF006100"/>
       </font>
       <fill>
@@ -4446,886 +4298,6 @@
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
           <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749992370372631"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749992370372631"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749992370372631"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749992370372631"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749992370372631"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749992370372631"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749992370372631"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="-0.24994659260841701"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="4" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="3" tint="0.79998168889431442"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="2" tint="-0.749992370372631"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="2" tint="-9.9978637043366805E-2"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF006100"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFC6EFCE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C6500"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFEB9C"/>
         </patternFill>
       </fill>
     </dxf>
@@ -6140,8 +5112,8 @@
   <dimension ref="A1:K310"/>
   <sheetViews>
     <sheetView tabSelected="1" showOutlineSymbols="0" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C57" sqref="C57"/>
+      <pane ySplit="3" topLeftCell="A16" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I16" sqref="I16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="7" x14ac:dyDescent="0"/>
@@ -6161,34 +5133,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="43" customFormat="1" ht="72" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="111"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="116"/>
     </row>
     <row r="2" spans="1:11" s="42" customFormat="1" ht="18">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="111" t="s">
         <v>83</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="108"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="113"/>
     </row>
     <row r="3" spans="1:11" s="41" customFormat="1" ht="25" customHeight="1">
       <c r="A3" s="38" t="s">
@@ -6510,31 +5482,31 @@
       <c r="B12" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C12" s="112" t="s">
+      <c r="C12" s="106" t="s">
         <v>164</v>
       </c>
-      <c r="D12" s="113" t="s">
+      <c r="D12" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E12" s="113" t="s">
+      <c r="E12" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="F12" s="114" t="s">
+      <c r="F12" s="108" t="s">
         <v>55</v>
       </c>
-      <c r="G12" s="114">
+      <c r="G12" s="108">
         <v>41390</v>
       </c>
-      <c r="H12" s="114">
+      <c r="H12" s="108">
         <v>41450</v>
       </c>
-      <c r="I12" s="113" t="s">
+      <c r="I12" s="107" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="113" t="s">
+      <c r="J12" s="107" t="s">
         <v>33</v>
       </c>
-      <c r="K12" s="115" t="s">
+      <c r="K12" s="109" t="s">
         <v>321</v>
       </c>
     </row>
@@ -6543,31 +5515,31 @@
       <c r="B13" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C13" s="112" t="s">
+      <c r="C13" s="106" t="s">
         <v>327</v>
       </c>
-      <c r="D13" s="113" t="s">
+      <c r="D13" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E13" s="113" t="s">
+      <c r="E13" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="F13" s="114" t="s">
+      <c r="F13" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="G13" s="114">
+      <c r="G13" s="108">
         <v>41450</v>
       </c>
-      <c r="H13" s="114">
+      <c r="H13" s="108">
         <v>41450</v>
       </c>
-      <c r="I13" s="113" t="s">
+      <c r="I13" s="107" t="s">
         <v>5</v>
       </c>
-      <c r="J13" s="113" t="s">
+      <c r="J13" s="107" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="115" t="s">
+      <c r="K13" s="109" t="s">
         <v>325</v>
       </c>
     </row>
@@ -6576,58 +5548,62 @@
       <c r="B14" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="C14" s="112" t="s">
+      <c r="C14" s="106" t="s">
         <v>335</v>
       </c>
-      <c r="D14" s="113" t="s">
+      <c r="D14" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E14" s="113" t="s">
+      <c r="E14" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="F14" s="114" t="s">
+      <c r="F14" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="G14" s="114" t="s">
+      <c r="G14" s="108" t="s">
         <v>336</v>
       </c>
-      <c r="H14" s="114">
+      <c r="H14" s="108">
         <v>41450</v>
       </c>
-      <c r="I14" s="113" t="s">
-        <v>221</v>
-      </c>
-      <c r="J14" s="113"/>
-      <c r="K14" s="115"/>
+      <c r="I14" s="107" t="s">
+        <v>5</v>
+      </c>
+      <c r="J14" s="107" t="s">
+        <v>31</v>
+      </c>
+      <c r="K14" s="109"/>
     </row>
     <row r="15" spans="1:11" s="70" customFormat="1" ht="90">
       <c r="A15" s="69"/>
       <c r="B15" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C15" s="112" t="s">
+      <c r="C15" s="106" t="s">
         <v>328</v>
       </c>
-      <c r="D15" s="113" t="s">
+      <c r="D15" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="113" t="s">
+      <c r="E15" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="F15" s="114" t="s">
+      <c r="F15" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="114">
+      <c r="G15" s="108">
         <v>41453</v>
       </c>
-      <c r="H15" s="114">
+      <c r="H15" s="108">
         <v>41450</v>
       </c>
-      <c r="I15" s="113" t="s">
-        <v>221</v>
-      </c>
-      <c r="J15" s="113"/>
-      <c r="K15" s="115" t="s">
+      <c r="I15" s="107" t="s">
+        <v>5</v>
+      </c>
+      <c r="J15" s="107" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="109" t="s">
         <v>326</v>
       </c>
     </row>
@@ -6636,29 +5612,29 @@
       <c r="B16" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="C16" s="112" t="s">
+      <c r="C16" s="106" t="s">
         <v>337</v>
       </c>
-      <c r="D16" s="113" t="s">
+      <c r="D16" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E16" s="113" t="s">
+      <c r="E16" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="F16" s="114" t="s">
+      <c r="F16" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="G16" s="114">
+      <c r="G16" s="108">
         <v>41458</v>
       </c>
-      <c r="H16" s="114">
+      <c r="H16" s="108">
         <v>41450</v>
       </c>
-      <c r="I16" s="113" t="s">
+      <c r="I16" s="107" t="s">
         <v>221</v>
       </c>
-      <c r="J16" s="113"/>
-      <c r="K16" s="115" t="s">
+      <c r="J16" s="107"/>
+      <c r="K16" s="109" t="s">
         <v>341</v>
       </c>
     </row>
@@ -6667,29 +5643,29 @@
       <c r="B17" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C17" s="112" t="s">
+      <c r="C17" s="106" t="s">
         <v>329</v>
       </c>
-      <c r="D17" s="113" t="s">
+      <c r="D17" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E17" s="113" t="s">
+      <c r="E17" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="F17" s="114" t="s">
+      <c r="F17" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="G17" s="114">
+      <c r="G17" s="108">
         <v>41457</v>
       </c>
-      <c r="H17" s="114">
+      <c r="H17" s="108">
         <v>41450</v>
       </c>
-      <c r="I17" s="113" t="s">
+      <c r="I17" s="107" t="s">
         <v>221</v>
       </c>
-      <c r="J17" s="113"/>
-      <c r="K17" s="115" t="s">
+      <c r="J17" s="107"/>
+      <c r="K17" s="109" t="s">
         <v>334</v>
       </c>
     </row>
@@ -6698,29 +5674,29 @@
       <c r="B18" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C18" s="112" t="s">
+      <c r="C18" s="106" t="s">
         <v>330</v>
       </c>
-      <c r="D18" s="113" t="s">
+      <c r="D18" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E18" s="113" t="s">
+      <c r="E18" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="F18" s="114" t="s">
+      <c r="F18" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="G18" s="114">
+      <c r="G18" s="108">
         <v>41457</v>
       </c>
-      <c r="H18" s="114">
+      <c r="H18" s="108">
         <v>41450</v>
       </c>
-      <c r="I18" s="113" t="s">
+      <c r="I18" s="107" t="s">
         <v>221</v>
       </c>
-      <c r="J18" s="113"/>
-      <c r="K18" s="115" t="s">
+      <c r="J18" s="107"/>
+      <c r="K18" s="109" t="s">
         <v>331</v>
       </c>
     </row>
@@ -6729,29 +5705,29 @@
       <c r="B19" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C19" s="112" t="s">
+      <c r="C19" s="106" t="s">
         <v>332</v>
       </c>
-      <c r="D19" s="113" t="s">
+      <c r="D19" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E19" s="113" t="s">
+      <c r="E19" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="F19" s="114" t="s">
+      <c r="F19" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="114">
+      <c r="G19" s="108">
         <v>41457</v>
       </c>
-      <c r="H19" s="114">
+      <c r="H19" s="108">
         <v>41450</v>
       </c>
-      <c r="I19" s="113" t="s">
+      <c r="I19" s="107" t="s">
         <v>221</v>
       </c>
-      <c r="J19" s="113"/>
-      <c r="K19" s="115" t="s">
+      <c r="J19" s="107"/>
+      <c r="K19" s="109" t="s">
         <v>333</v>
       </c>
     </row>
@@ -6760,29 +5736,29 @@
       <c r="B20" s="55" t="s">
         <v>85</v>
       </c>
-      <c r="C20" s="112" t="s">
+      <c r="C20" s="106" t="s">
         <v>338</v>
       </c>
-      <c r="D20" s="113" t="s">
+      <c r="D20" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E20" s="113" t="s">
+      <c r="E20" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="F20" s="114" t="s">
+      <c r="F20" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="114">
+      <c r="G20" s="108">
         <v>41459</v>
       </c>
-      <c r="H20" s="114">
+      <c r="H20" s="108">
         <v>41450</v>
       </c>
-      <c r="I20" s="113" t="s">
+      <c r="I20" s="107" t="s">
         <v>221</v>
       </c>
-      <c r="J20" s="113"/>
-      <c r="K20" s="115" t="s">
+      <c r="J20" s="107"/>
+      <c r="K20" s="109" t="s">
         <v>339</v>
       </c>
     </row>
@@ -6791,29 +5767,29 @@
       <c r="B21" s="59" t="s">
         <v>84</v>
       </c>
-      <c r="C21" s="112" t="s">
+      <c r="C21" s="106" t="s">
         <v>322</v>
       </c>
-      <c r="D21" s="113" t="s">
+      <c r="D21" s="107" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="113" t="s">
+      <c r="E21" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="F21" s="114" t="s">
+      <c r="F21" s="108" t="s">
         <v>56</v>
       </c>
-      <c r="G21" s="114">
+      <c r="G21" s="108">
         <v>41460</v>
       </c>
-      <c r="H21" s="114">
+      <c r="H21" s="108">
         <v>41450</v>
       </c>
-      <c r="I21" s="113" t="s">
+      <c r="I21" s="107" t="s">
         <v>221</v>
       </c>
-      <c r="J21" s="113"/>
-      <c r="K21" s="115" t="s">
+      <c r="J21" s="107"/>
+      <c r="K21" s="109" t="s">
         <v>340</v>
       </c>
     </row>
@@ -6844,7 +5820,7 @@
         <v>6</v>
       </c>
       <c r="J22" s="73"/>
-      <c r="K22" s="116" t="s">
+      <c r="K22" s="110" t="s">
         <v>137</v>
       </c>
     </row>
@@ -11350,318 +10326,318 @@
     <mergeCell ref="A1:K1"/>
   </mergeCells>
   <conditionalFormatting sqref="I6:I13 I15 I17:I20 I22:I310">
-    <cfRule type="containsText" dxfId="194" priority="160" operator="containsText" text="PITCH">
+    <cfRule type="containsText" dxfId="180" priority="160" operator="containsText" text="PITCH">
       <formula>NOT(ISERROR(SEARCH("PITCH",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="193" priority="161" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="179" priority="161" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="192" priority="162" operator="containsText" text="ON TRACK">
+    <cfRule type="containsText" dxfId="178" priority="162" operator="containsText" text="ON TRACK">
       <formula>NOT(ISERROR(SEARCH("ON TRACK",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="191" priority="163" operator="containsText" text="ATTENTION">
+    <cfRule type="containsText" dxfId="177" priority="163" operator="containsText" text="ATTENTION">
       <formula>NOT(ISERROR(SEARCH("ATTENTION",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="190" priority="164" operator="containsText" text="OFF TRACK">
+    <cfRule type="containsText" dxfId="176" priority="164" operator="containsText" text="OFF TRACK">
       <formula>NOT(ISERROR(SEARCH("OFF TRACK",I6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4:A13 A22:A310 A19 A15">
-    <cfRule type="cellIs" dxfId="189" priority="457" operator="equal">
+    <cfRule type="cellIs" dxfId="175" priority="457" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="188" priority="458" operator="equal">
+    <cfRule type="cellIs" dxfId="174" priority="458" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="187" priority="459" operator="equal">
+    <cfRule type="cellIs" dxfId="173" priority="459" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J6:J13 J22:J310 J19 J15">
-    <cfRule type="containsText" dxfId="186" priority="119" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="172" priority="119" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="185" priority="120" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="171" priority="120" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="184" priority="121" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="170" priority="121" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J6)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="183" priority="122" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="169" priority="122" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J6,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I5">
-    <cfRule type="containsText" dxfId="182" priority="113" operator="containsText" text="PITCH">
+    <cfRule type="containsText" dxfId="168" priority="113" operator="containsText" text="PITCH">
       <formula>NOT(ISERROR(SEARCH("PITCH",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="181" priority="114" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="167" priority="114" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="180" priority="116" operator="containsText" text="ATTENTION">
+    <cfRule type="containsText" dxfId="166" priority="116" operator="containsText" text="ATTENTION">
       <formula>NOT(ISERROR(SEARCH("ATTENTION",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="179" priority="117" operator="containsText" text="OFF TRACK">
+    <cfRule type="containsText" dxfId="165" priority="117" operator="containsText" text="OFF TRACK">
       <formula>NOT(ISERROR(SEARCH("OFF TRACK",I4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J5">
-    <cfRule type="containsText" dxfId="178" priority="109" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="164" priority="109" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="177" priority="110" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="163" priority="110" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="176" priority="111" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="162" priority="111" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J4)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="175" priority="112" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="161" priority="112" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J4,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I2 I4:I13 I15 I17:I20 I22:I1048576">
-    <cfRule type="containsText" dxfId="174" priority="108" operator="containsText" text="Planned">
+    <cfRule type="containsText" dxfId="160" priority="108" operator="containsText" text="Planned">
       <formula>NOT(ISERROR(SEARCH("Planned",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I3">
-    <cfRule type="containsText" dxfId="173" priority="107" operator="containsText" text="Planned">
+    <cfRule type="containsText" dxfId="159" priority="107" operator="containsText" text="Planned">
       <formula>NOT(ISERROR(SEARCH("Planned",I3)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I13 I15 I17:I20 I22:I1048576">
-    <cfRule type="containsText" dxfId="172" priority="106" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="158" priority="106" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A20">
-    <cfRule type="cellIs" dxfId="171" priority="89" operator="equal">
+    <cfRule type="cellIs" dxfId="157" priority="89" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="170" priority="90" operator="equal">
+    <cfRule type="cellIs" dxfId="156" priority="90" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="169" priority="91" operator="equal">
+    <cfRule type="cellIs" dxfId="155" priority="91" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J20">
-    <cfRule type="containsText" dxfId="168" priority="80" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="154" priority="80" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="167" priority="81" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="153" priority="81" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J20)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="166" priority="82" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="152" priority="82" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J20)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="165" priority="83" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="151" priority="83" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J20,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A18">
-    <cfRule type="cellIs" dxfId="164" priority="75" operator="equal">
+    <cfRule type="cellIs" dxfId="150" priority="75" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="163" priority="76" operator="equal">
+    <cfRule type="cellIs" dxfId="149" priority="76" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="162" priority="77" operator="equal">
+    <cfRule type="cellIs" dxfId="148" priority="77" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J18">
-    <cfRule type="containsText" dxfId="161" priority="66" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="147" priority="66" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="160" priority="67" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="146" priority="67" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J18)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="159" priority="68" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="145" priority="68" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J18)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="158" priority="69" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="144" priority="69" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J18,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A17">
-    <cfRule type="cellIs" dxfId="157" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="143" priority="61" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="156" priority="62" operator="equal">
+    <cfRule type="cellIs" dxfId="142" priority="62" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="155" priority="63" operator="equal">
+    <cfRule type="cellIs" dxfId="141" priority="63" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17">
-    <cfRule type="containsText" dxfId="154" priority="52" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="140" priority="52" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="153" priority="53" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="139" priority="53" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="152" priority="54" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="138" priority="54" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="151" priority="55" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="137" priority="55" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J17,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A14">
-    <cfRule type="cellIs" dxfId="150" priority="40" operator="equal">
+    <cfRule type="cellIs" dxfId="136" priority="40" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="149" priority="41" operator="equal">
+    <cfRule type="cellIs" dxfId="135" priority="41" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="148" priority="42" operator="equal">
+    <cfRule type="cellIs" dxfId="134" priority="42" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14">
-    <cfRule type="containsText" dxfId="147" priority="36" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="133" priority="36" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="146" priority="37" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="132" priority="37" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="145" priority="38" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="131" priority="38" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J14)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="144" priority="39" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="130" priority="39" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J14,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="143" priority="31" operator="containsText" text="PITCH">
+    <cfRule type="containsText" dxfId="129" priority="31" operator="containsText" text="PITCH">
       <formula>NOT(ISERROR(SEARCH("PITCH",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="142" priority="32" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="128" priority="32" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="141" priority="33" operator="containsText" text="ON TRACK">
+    <cfRule type="containsText" dxfId="127" priority="33" operator="containsText" text="ON TRACK">
       <formula>NOT(ISERROR(SEARCH("ON TRACK",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="140" priority="34" operator="containsText" text="ATTENTION">
+    <cfRule type="containsText" dxfId="126" priority="34" operator="containsText" text="ATTENTION">
       <formula>NOT(ISERROR(SEARCH("ATTENTION",I14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="139" priority="35" operator="containsText" text="OFF TRACK">
+    <cfRule type="containsText" dxfId="125" priority="35" operator="containsText" text="OFF TRACK">
       <formula>NOT(ISERROR(SEARCH("OFF TRACK",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="138" priority="30" operator="containsText" text="Planned">
+    <cfRule type="containsText" dxfId="124" priority="30" operator="containsText" text="Planned">
       <formula>NOT(ISERROR(SEARCH("Planned",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I14">
-    <cfRule type="containsText" dxfId="137" priority="29" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="123" priority="29" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",I14)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A16">
-    <cfRule type="cellIs" dxfId="136" priority="26" operator="equal">
+    <cfRule type="cellIs" dxfId="122" priority="26" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="135" priority="27" operator="equal">
+    <cfRule type="cellIs" dxfId="121" priority="27" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="134" priority="28" operator="equal">
+    <cfRule type="cellIs" dxfId="120" priority="28" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J16">
-    <cfRule type="containsText" dxfId="133" priority="22" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="119" priority="22" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="132" priority="23" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="118" priority="23" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="131" priority="24" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="117" priority="24" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J16)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="130" priority="25" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="116" priority="25" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J16,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="containsText" dxfId="129" priority="17" operator="containsText" text="PITCH">
+    <cfRule type="containsText" dxfId="115" priority="17" operator="containsText" text="PITCH">
       <formula>NOT(ISERROR(SEARCH("PITCH",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="128" priority="18" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="114" priority="18" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="127" priority="19" operator="containsText" text="ON TRACK">
+    <cfRule type="containsText" dxfId="113" priority="19" operator="containsText" text="ON TRACK">
       <formula>NOT(ISERROR(SEARCH("ON TRACK",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="126" priority="20" operator="containsText" text="ATTENTION">
+    <cfRule type="containsText" dxfId="112" priority="20" operator="containsText" text="ATTENTION">
       <formula>NOT(ISERROR(SEARCH("ATTENTION",I16)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="125" priority="21" operator="containsText" text="OFF TRACK">
+    <cfRule type="containsText" dxfId="111" priority="21" operator="containsText" text="OFF TRACK">
       <formula>NOT(ISERROR(SEARCH("OFF TRACK",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="containsText" dxfId="124" priority="16" operator="containsText" text="Planned">
+    <cfRule type="containsText" dxfId="110" priority="16" operator="containsText" text="Planned">
       <formula>NOT(ISERROR(SEARCH("Planned",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I16">
-    <cfRule type="containsText" dxfId="123" priority="15" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="109" priority="15" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",I16)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="27" priority="10" operator="containsText" text="PITCH">
+    <cfRule type="containsText" dxfId="108" priority="10" operator="containsText" text="PITCH">
       <formula>NOT(ISERROR(SEARCH("PITCH",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="26" priority="11" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="107" priority="11" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="25" priority="12" operator="containsText" text="ON TRACK">
+    <cfRule type="containsText" dxfId="106" priority="12" operator="containsText" text="ON TRACK">
       <formula>NOT(ISERROR(SEARCH("ON TRACK",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="24" priority="13" operator="containsText" text="ATTENTION">
+    <cfRule type="containsText" dxfId="105" priority="13" operator="containsText" text="ATTENTION">
       <formula>NOT(ISERROR(SEARCH("ATTENTION",I21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="23" priority="14" operator="containsText" text="OFF TRACK">
+    <cfRule type="containsText" dxfId="104" priority="14" operator="containsText" text="OFF TRACK">
       <formula>NOT(ISERROR(SEARCH("OFF TRACK",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="17" priority="9" operator="containsText" text="Planned">
+    <cfRule type="containsText" dxfId="103" priority="9" operator="containsText" text="Planned">
       <formula>NOT(ISERROR(SEARCH("Planned",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I21">
-    <cfRule type="containsText" dxfId="15" priority="8" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="102" priority="8" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",I21)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A21">
-    <cfRule type="cellIs" dxfId="13" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="101" priority="5" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="12" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="100" priority="6" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="11" priority="7" operator="equal">
+    <cfRule type="cellIs" dxfId="99" priority="7" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J21">
-    <cfRule type="containsText" dxfId="7" priority="1" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="98" priority="1" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="6" priority="2" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="97" priority="2" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J21)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="5" priority="3" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="96" priority="3" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J21)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="4" priority="4" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="95" priority="4" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J21,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11725,34 +10701,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="43" customFormat="1" ht="72" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="111"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="116"/>
     </row>
     <row r="2" spans="1:11" s="42" customFormat="1" ht="18">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="111" t="s">
         <v>133</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="108"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="113"/>
     </row>
     <row r="3" spans="1:11" s="41" customFormat="1" ht="25" customHeight="1">
       <c r="A3" s="38" t="s">
@@ -16709,213 +15685,213 @@
     <mergeCell ref="A2:K2"/>
   </mergeCells>
   <conditionalFormatting sqref="I66:I305 I6:I55">
-    <cfRule type="containsText" dxfId="122" priority="77" operator="containsText" text="PITCH">
+    <cfRule type="containsText" dxfId="94" priority="77" operator="containsText" text="PITCH">
       <formula>NOT(ISERROR(SEARCH("PITCH",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="121" priority="78" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="93" priority="78" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="120" priority="80" operator="containsText" text="ATTENTION">
+    <cfRule type="containsText" dxfId="92" priority="80" operator="containsText" text="ATTENTION">
       <formula>NOT(ISERROR(SEARCH("ATTENTION",I6)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="119" priority="81" operator="containsText" text="OFF TRACK">
+    <cfRule type="containsText" dxfId="91" priority="81" operator="containsText" text="OFF TRACK">
       <formula>NOT(ISERROR(SEARCH("OFF TRACK",I6)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A63:A305 A6:A55">
-    <cfRule type="cellIs" dxfId="118" priority="82" operator="equal">
+    <cfRule type="cellIs" dxfId="90" priority="82" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="117" priority="83" operator="equal">
+    <cfRule type="cellIs" dxfId="89" priority="83" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="116" priority="84" operator="equal">
+    <cfRule type="cellIs" dxfId="88" priority="84" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="F66:F305">
-    <cfRule type="cellIs" dxfId="115" priority="76" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="87" priority="76" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J14:J16 J66:J305 J21:J55">
-    <cfRule type="containsText" dxfId="114" priority="72" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="86" priority="72" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="113" priority="73" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="85" priority="73" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J14)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="112" priority="74" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="84" priority="74" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J14)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="111" priority="75" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="83" priority="75" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J14,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J17:J20">
-    <cfRule type="containsText" dxfId="110" priority="63" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="82" priority="63" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="109" priority="64" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="81" priority="64" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J17)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="108" priority="65" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="80" priority="65" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J17)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="107" priority="66" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="79" priority="66" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J17,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I3 I66:I1048576 I6:I55">
-    <cfRule type="containsText" dxfId="106" priority="62" operator="containsText" text="Planned">
+    <cfRule type="containsText" dxfId="78" priority="62" operator="containsText" text="Planned">
       <formula>NOT(ISERROR(SEARCH("Planned",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5">
-    <cfRule type="cellIs" dxfId="105" priority="59" operator="equal">
+    <cfRule type="cellIs" dxfId="77" priority="59" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="104" priority="60" operator="equal">
+    <cfRule type="cellIs" dxfId="76" priority="60" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="103" priority="61" operator="equal">
+    <cfRule type="cellIs" dxfId="75" priority="61" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A4">
-    <cfRule type="cellIs" dxfId="102" priority="46" operator="equal">
+    <cfRule type="cellIs" dxfId="74" priority="46" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="101" priority="47" operator="equal">
+    <cfRule type="cellIs" dxfId="73" priority="47" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="100" priority="48" operator="equal">
+    <cfRule type="cellIs" dxfId="72" priority="48" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J4:J13">
-    <cfRule type="containsText" dxfId="99" priority="32" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="71" priority="32" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="98" priority="33" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="70" priority="33" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="97" priority="34" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="69" priority="34" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J4)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="96" priority="35" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="68" priority="35" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J4,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I5">
-    <cfRule type="containsText" dxfId="95" priority="27" operator="containsText" text="PITCH">
+    <cfRule type="containsText" dxfId="67" priority="27" operator="containsText" text="PITCH">
       <formula>NOT(ISERROR(SEARCH("PITCH",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="94" priority="28" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="66" priority="28" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="93" priority="29" operator="containsText" text="ON TRACK">
+    <cfRule type="containsText" dxfId="65" priority="29" operator="containsText" text="ON TRACK">
       <formula>NOT(ISERROR(SEARCH("ON TRACK",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="92" priority="30" operator="containsText" text="ATTENTION">
+    <cfRule type="containsText" dxfId="64" priority="30" operator="containsText" text="ATTENTION">
       <formula>NOT(ISERROR(SEARCH("ATTENTION",I4)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="91" priority="31" operator="containsText" text="OFF TRACK">
+    <cfRule type="containsText" dxfId="63" priority="31" operator="containsText" text="OFF TRACK">
       <formula>NOT(ISERROR(SEARCH("OFF TRACK",I4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I4:I5">
-    <cfRule type="containsText" dxfId="90" priority="26" operator="containsText" text="Planned">
+    <cfRule type="containsText" dxfId="62" priority="26" operator="containsText" text="Planned">
       <formula>NOT(ISERROR(SEARCH("Planned",I4)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I56:I62">
-    <cfRule type="containsText" dxfId="89" priority="18" operator="containsText" text="PITCH">
+    <cfRule type="containsText" dxfId="61" priority="18" operator="containsText" text="PITCH">
       <formula>NOT(ISERROR(SEARCH("PITCH",I56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="88" priority="19" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="60" priority="19" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",I56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="87" priority="20" operator="containsText" text="ON TRACK">
+    <cfRule type="containsText" dxfId="59" priority="20" operator="containsText" text="ON TRACK">
       <formula>NOT(ISERROR(SEARCH("ON TRACK",I56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="86" priority="21" operator="containsText" text="ATTENTION">
+    <cfRule type="containsText" dxfId="58" priority="21" operator="containsText" text="ATTENTION">
       <formula>NOT(ISERROR(SEARCH("ATTENTION",I56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="85" priority="22" operator="containsText" text="OFF TRACK">
+    <cfRule type="containsText" dxfId="57" priority="22" operator="containsText" text="OFF TRACK">
       <formula>NOT(ISERROR(SEARCH("OFF TRACK",I56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A56:A62">
-    <cfRule type="cellIs" dxfId="84" priority="23" operator="equal">
+    <cfRule type="cellIs" dxfId="56" priority="23" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="83" priority="24" operator="equal">
+    <cfRule type="cellIs" dxfId="55" priority="24" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="82" priority="25" operator="equal">
+    <cfRule type="cellIs" dxfId="54" priority="25" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J56:J62">
-    <cfRule type="containsText" dxfId="81" priority="13" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="53" priority="13" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="80" priority="14" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="52" priority="14" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J56)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="79" priority="15" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="51" priority="15" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J56)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="78" priority="16" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="50" priority="16" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J56,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I56:I62">
-    <cfRule type="containsText" dxfId="77" priority="12" operator="containsText" text="Planned">
+    <cfRule type="containsText" dxfId="49" priority="12" operator="containsText" text="Planned">
       <formula>NOT(ISERROR(SEARCH("Planned",I56)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63:I65">
-    <cfRule type="containsText" dxfId="76" priority="7" operator="containsText" text="PITCH">
+    <cfRule type="containsText" dxfId="48" priority="7" operator="containsText" text="PITCH">
       <formula>NOT(ISERROR(SEARCH("PITCH",I63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="75" priority="9" operator="containsText" text="ON TRACK">
+    <cfRule type="containsText" dxfId="47" priority="9" operator="containsText" text="ON TRACK">
       <formula>NOT(ISERROR(SEARCH("ON TRACK",I63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="74" priority="10" operator="containsText" text="ATTENTION">
+    <cfRule type="containsText" dxfId="46" priority="10" operator="containsText" text="ATTENTION">
       <formula>NOT(ISERROR(SEARCH("ATTENTION",I63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="73" priority="11" operator="containsText" text="OFF TRACK">
+    <cfRule type="containsText" dxfId="45" priority="11" operator="containsText" text="OFF TRACK">
       <formula>NOT(ISERROR(SEARCH("OFF TRACK",I63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="J63:J65">
-    <cfRule type="containsText" dxfId="72" priority="3" operator="containsText" text="SUBMITTED">
+    <cfRule type="containsText" dxfId="44" priority="3" operator="containsText" text="SUBMITTED">
       <formula>NOT(ISERROR(SEARCH("SUBMITTED",J63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="71" priority="4" operator="containsText" text="APPROVED">
+    <cfRule type="containsText" dxfId="43" priority="4" operator="containsText" text="APPROVED">
       <formula>NOT(ISERROR(SEARCH("APPROVED",J63)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="70" priority="5" operator="containsText" text="HOLDING">
+    <cfRule type="containsText" dxfId="42" priority="5" operator="containsText" text="HOLDING">
       <formula>NOT(ISERROR(SEARCH("HOLDING",J63)))</formula>
     </cfRule>
-    <cfRule type="beginsWith" dxfId="69" priority="6" operator="beginsWith" text="DECLINED">
+    <cfRule type="beginsWith" dxfId="41" priority="6" operator="beginsWith" text="DECLINED">
       <formula>LEFT(J63,LEN("DECLINED"))="DECLINED"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I63:I65">
-    <cfRule type="containsText" dxfId="68" priority="2" operator="containsText" text="Planned">
+    <cfRule type="containsText" dxfId="40" priority="2" operator="containsText" text="Planned">
       <formula>NOT(ISERROR(SEARCH("Planned",I63)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="67" priority="1" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="39" priority="1" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1:K1048576">
-    <cfRule type="containsText" dxfId="66" priority="8" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="38" priority="8" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",A1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -16975,36 +15951,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="43" customFormat="1" ht="47" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
-      <c r="L1" s="111"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="116"/>
     </row>
     <row r="2" spans="1:12" s="42" customFormat="1" ht="18">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="111" t="s">
         <v>230</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="108"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="113"/>
     </row>
     <row r="3" spans="1:12" s="41" customFormat="1" ht="32" customHeight="1">
       <c r="A3" s="38" t="s">
@@ -17938,47 +16914,47 @@
     <mergeCell ref="A2:L2"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:A36">
-    <cfRule type="cellIs" dxfId="65" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="37" priority="11" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="64" priority="12" operator="equal">
+    <cfRule type="cellIs" dxfId="36" priority="12" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="63" priority="13" operator="equal">
+    <cfRule type="cellIs" dxfId="35" priority="13" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="62" priority="4" operator="containsText" text="ON HOLD">
+    <cfRule type="containsText" dxfId="34" priority="4" operator="containsText" text="ON HOLD">
       <formula>NOT(ISERROR(SEARCH("ON HOLD",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="61" priority="5" operator="containsText" text="IN DESIGN">
+    <cfRule type="containsText" dxfId="33" priority="5" operator="containsText" text="IN DESIGN">
       <formula>NOT(ISERROR(SEARCH("IN DESIGN",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="60" priority="6" operator="containsText" text="IN DISCUSSION">
+    <cfRule type="containsText" dxfId="32" priority="6" operator="containsText" text="IN DISCUSSION">
       <formula>NOT(ISERROR(SEARCH("IN DISCUSSION",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="59" priority="7" operator="containsText" text="OFF TRACK">
+    <cfRule type="containsText" dxfId="31" priority="7" operator="containsText" text="OFF TRACK">
       <formula>NOT(ISERROR(SEARCH("OFF TRACK",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="58" priority="8" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="30" priority="8" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="57" priority="9" operator="containsText" text="ATTENTION">
+    <cfRule type="containsText" dxfId="29" priority="9" operator="containsText" text="ATTENTION">
       <formula>NOT(ISERROR(SEARCH("ATTENTION",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="56" priority="10" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="28" priority="10" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="A37">
-    <cfRule type="cellIs" dxfId="55" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="27" priority="1" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="54" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="26" priority="2" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="53" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="25" priority="3" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18078,36 +17054,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" s="43" customFormat="1" ht="47" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="110"/>
-      <c r="I1" s="110"/>
-      <c r="J1" s="110"/>
-      <c r="K1" s="110"/>
-      <c r="L1" s="111"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="115"/>
+      <c r="I1" s="115"/>
+      <c r="J1" s="115"/>
+      <c r="K1" s="115"/>
+      <c r="L1" s="116"/>
     </row>
     <row r="2" spans="1:12" s="42" customFormat="1" ht="18">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="111" t="s">
         <v>219</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="107"/>
-      <c r="I2" s="107"/>
-      <c r="J2" s="107"/>
-      <c r="K2" s="107"/>
-      <c r="L2" s="108"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="112"/>
+      <c r="I2" s="112"/>
+      <c r="J2" s="112"/>
+      <c r="K2" s="112"/>
+      <c r="L2" s="113"/>
     </row>
     <row r="3" spans="1:12" s="41" customFormat="1" ht="32" customHeight="1">
       <c r="A3" s="38" t="s">
@@ -18485,36 +17461,36 @@
     <mergeCell ref="A2:L2"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:A19">
-    <cfRule type="cellIs" dxfId="50" priority="19" operator="equal">
+    <cfRule type="cellIs" dxfId="22" priority="19" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="49" priority="20" operator="equal">
+    <cfRule type="cellIs" dxfId="21" priority="20" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="48" priority="21" operator="equal">
+    <cfRule type="cellIs" dxfId="20" priority="21" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="containsText" dxfId="47" priority="1" operator="containsText" text="ON HOLD">
+    <cfRule type="containsText" dxfId="19" priority="1" operator="containsText" text="ON HOLD">
       <formula>NOT(ISERROR(SEARCH("ON HOLD",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="46" priority="2" operator="containsText" text="IN DESIGN">
+    <cfRule type="containsText" dxfId="18" priority="2" operator="containsText" text="IN DESIGN">
       <formula>NOT(ISERROR(SEARCH("IN DESIGN",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="45" priority="3" operator="containsText" text="IN DISCUSSION">
+    <cfRule type="containsText" dxfId="17" priority="3" operator="containsText" text="IN DISCUSSION">
       <formula>NOT(ISERROR(SEARCH("IN DISCUSSION",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="44" priority="4" operator="containsText" text="OFF TRACK">
+    <cfRule type="containsText" dxfId="16" priority="4" operator="containsText" text="OFF TRACK">
       <formula>NOT(ISERROR(SEARCH("OFF TRACK",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="43" priority="5" operator="containsText" text="COMPLETE">
+    <cfRule type="containsText" dxfId="15" priority="5" operator="containsText" text="COMPLETE">
       <formula>NOT(ISERROR(SEARCH("COMPLETE",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="42" priority="6" operator="containsText" text="ATTENTION">
+    <cfRule type="containsText" dxfId="14" priority="6" operator="containsText" text="ATTENTION">
       <formula>NOT(ISERROR(SEARCH("ATTENTION",I1)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="41" priority="7" operator="containsText" text="IN PROGRESS">
+    <cfRule type="containsText" dxfId="13" priority="7" operator="containsText" text="IN PROGRESS">
       <formula>NOT(ISERROR(SEARCH("IN PROGRESS",I1)))</formula>
     </cfRule>
   </conditionalFormatting>
@@ -18611,28 +17587,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="43" customFormat="1" ht="47" customHeight="1">
-      <c r="A1" s="109" t="s">
+      <c r="A1" s="114" t="s">
         <v>26</v>
       </c>
-      <c r="B1" s="110"/>
-      <c r="C1" s="110"/>
-      <c r="D1" s="110"/>
-      <c r="E1" s="110"/>
-      <c r="F1" s="110"/>
-      <c r="G1" s="110"/>
-      <c r="H1" s="111"/>
+      <c r="B1" s="115"/>
+      <c r="C1" s="115"/>
+      <c r="D1" s="115"/>
+      <c r="E1" s="115"/>
+      <c r="F1" s="115"/>
+      <c r="G1" s="115"/>
+      <c r="H1" s="116"/>
     </row>
     <row r="2" spans="1:8" s="42" customFormat="1" ht="18">
-      <c r="A2" s="106" t="s">
+      <c r="A2" s="111" t="s">
         <v>219</v>
       </c>
-      <c r="B2" s="107"/>
-      <c r="C2" s="107"/>
-      <c r="D2" s="107"/>
-      <c r="E2" s="107"/>
-      <c r="F2" s="107"/>
-      <c r="G2" s="107"/>
-      <c r="H2" s="108"/>
+      <c r="B2" s="112"/>
+      <c r="C2" s="112"/>
+      <c r="D2" s="112"/>
+      <c r="E2" s="112"/>
+      <c r="F2" s="112"/>
+      <c r="G2" s="112"/>
+      <c r="H2" s="113"/>
     </row>
     <row r="3" spans="1:8" s="41" customFormat="1" ht="32" customHeight="1">
       <c r="A3" s="39" t="s">
@@ -19216,13 +18192,13 @@
     <mergeCell ref="A2:H2"/>
   </mergeCells>
   <conditionalFormatting sqref="A4:B29">
-    <cfRule type="cellIs" dxfId="38" priority="9" operator="equal">
+    <cfRule type="cellIs" dxfId="10" priority="9" operator="equal">
       <formula>3</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="37" priority="10" operator="equal">
+    <cfRule type="cellIs" dxfId="9" priority="10" operator="equal">
       <formula>2</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="36" priority="11" operator="equal">
+    <cfRule type="cellIs" dxfId="8" priority="11" operator="equal">
       <formula>1</formula>
     </cfRule>
   </conditionalFormatting>
@@ -19557,36 +18533,36 @@
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="E6:E8">
-    <cfRule type="expression" dxfId="35" priority="358">
+    <cfRule type="expression" dxfId="7" priority="358">
       <formula>($G5=3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="34" priority="359">
+    <cfRule type="expression" dxfId="6" priority="359">
       <formula>($G5=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E2">
-    <cfRule type="expression" dxfId="33" priority="364">
+    <cfRule type="expression" dxfId="5" priority="364">
       <formula>($G3=3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="32" priority="365">
+    <cfRule type="expression" dxfId="4" priority="365">
       <formula>($G3=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E3">
-    <cfRule type="expression" dxfId="31" priority="366">
+    <cfRule type="expression" dxfId="3" priority="366">
       <formula>($G3=1)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1">
-    <cfRule type="expression" dxfId="30" priority="367">
+    <cfRule type="expression" dxfId="2" priority="367">
       <formula>($G1=3)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="E4:E5">
-    <cfRule type="expression" dxfId="29" priority="368">
+    <cfRule type="expression" dxfId="1" priority="368">
       <formula>($G4=3)</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="28" priority="369">
+    <cfRule type="expression" dxfId="0" priority="369">
       <formula>($G4=1)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>